<commit_message>
Added all time course data and a simple script to read it into a dataframe
</commit_message>
<xml_diff>
--- a/Experimental_Data.xlsx
+++ b/Experimental_Data.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,29 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Duncan\Documents\University\Grad Studies Year 1\IFN Summer 2018\IFN Pipeline\IFNmodeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1AF4D35B-8CB3-407A-A71B-C38149597AB8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{9AD0D326-6798-45AF-BFE0-4844E9030EDC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{5541B396-8A53-4390-86A0-578876AA7D92}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5652"/>
   </bookViews>
   <sheets>
     <sheet name="Experimental_Data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="6">
+  <si>
+    <t>Interferon</t>
+  </si>
   <si>
     <t>Dose (pM)</t>
-  </si>
-  <si>
-    <t>Interferon</t>
   </si>
   <si>
     <t>Alpha</t>
@@ -48,8 +43,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -57,16 +52,316 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -74,15 +369,204 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="42">
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -393,17 +877,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E394F2F3-AE6F-4818-8711-6CAE9CB455D9}">
-  <dimension ref="A1:G5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -429,11 +910,11 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2">
-        <v>10</v>
       </c>
       <c r="C2">
         <v>300</v>
@@ -442,86 +923,269 @@
         <v>150</v>
       </c>
       <c r="E2">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="F2">
-        <v>220</v>
+        <v>230</v>
       </c>
       <c r="G2">
-        <v>650</v>
+        <v>675</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
-      </c>
-      <c r="B3">
-        <v>10</v>
       </c>
       <c r="C3">
         <v>300</v>
       </c>
       <c r="D3">
-        <v>1100</v>
+        <v>1110</v>
       </c>
       <c r="E3">
-        <v>1200</v>
+        <v>1195</v>
       </c>
       <c r="F3">
-        <v>1500</v>
+        <v>1520</v>
       </c>
       <c r="G3">
-        <v>850</v>
+        <v>825</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
+      <c r="C4">
+        <v>90</v>
+      </c>
+      <c r="D4">
+        <v>110</v>
+      </c>
+      <c r="E4">
+        <v>150</v>
+      </c>
+      <c r="F4">
+        <v>110</v>
+      </c>
+      <c r="G4">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
         <v>10</v>
       </c>
-      <c r="C4">
-        <v>80</v>
-      </c>
-      <c r="D4">
-        <v>100</v>
-      </c>
-      <c r="E4">
-        <v>200</v>
-      </c>
-      <c r="F4">
-        <v>80</v>
-      </c>
-      <c r="G4">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="B5">
-        <v>10</v>
-      </c>
       <c r="C5">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="D5">
-        <v>300</v>
+        <v>315</v>
       </c>
       <c r="E5">
-        <v>300</v>
+        <v>340</v>
       </c>
       <c r="F5">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="G5">
-        <v>200</v>
+        <v>185</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>90</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>295</v>
+      </c>
+      <c r="D6">
+        <v>1510</v>
+      </c>
+      <c r="E6">
+        <v>1730</v>
+      </c>
+      <c r="F6">
+        <v>955</v>
+      </c>
+      <c r="G6">
+        <v>1220</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>90</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>295</v>
+      </c>
+      <c r="D7">
+        <v>1890</v>
+      </c>
+      <c r="E7">
+        <v>3900</v>
+      </c>
+      <c r="F7">
+        <v>5300</v>
+      </c>
+      <c r="G7">
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>90</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>90</v>
+      </c>
+      <c r="D8">
+        <v>340</v>
+      </c>
+      <c r="E8">
+        <v>380</v>
+      </c>
+      <c r="F8">
+        <v>185</v>
+      </c>
+      <c r="G8">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>90</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>90</v>
+      </c>
+      <c r="D9">
+        <v>270</v>
+      </c>
+      <c r="E9">
+        <v>525</v>
+      </c>
+      <c r="F9">
+        <v>995</v>
+      </c>
+      <c r="G9">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>600</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>275</v>
+      </c>
+      <c r="D10">
+        <v>3170</v>
+      </c>
+      <c r="E10">
+        <v>4505</v>
+      </c>
+      <c r="F10">
+        <v>3315</v>
+      </c>
+      <c r="G10">
+        <v>1685</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>600</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>275</v>
+      </c>
+      <c r="D11">
+        <v>625</v>
+      </c>
+      <c r="E11">
+        <v>10715</v>
+      </c>
+      <c r="F11">
+        <v>13333</v>
+      </c>
+      <c r="G11">
+        <v>6795</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>600</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>275</v>
+      </c>
+      <c r="D12">
+        <v>6120</v>
+      </c>
+      <c r="E12">
+        <v>770</v>
+      </c>
+      <c r="F12">
+        <v>1080</v>
+      </c>
+      <c r="G12">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>600</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>275</v>
+      </c>
+      <c r="D13">
+        <v>625</v>
+      </c>
+      <c r="E13">
+        <v>2345</v>
+      </c>
+      <c r="F13">
+        <v>4600</v>
+      </c>
+      <c r="G13">
+        <v>2270</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added all data as read off of experimental time course. File can be imported as a complete dataset.
</commit_message>
<xml_diff>
--- a/Experimental_Data.xlsx
+++ b/Experimental_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Duncan\Documents\University\Grad Studies Year 1\IFN Summer 2018\IFN Pipeline\IFNmodeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{9AD0D326-6798-45AF-BFE0-4844E9030EDC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{18092828-CC23-41AB-90D1-853C857A2D53}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5652"/>
   </bookViews>
@@ -881,7 +881,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1127,7 +1127,7 @@
         <v>275</v>
       </c>
       <c r="D11">
-        <v>625</v>
+        <v>6120</v>
       </c>
       <c r="E11">
         <v>10715</v>
@@ -1150,7 +1150,7 @@
         <v>275</v>
       </c>
       <c r="D12">
-        <v>6120</v>
+        <v>625</v>
       </c>
       <c r="E12">
         <v>770</v>

</xml_diff>